<commit_message>
3 pessoa se adapta a posição do coelho no mapa. O mapa em excel foi atualizado com os valores de X e Z corretos. O .txt esta com o mapa novo de 50x50.
</commit_message>
<xml_diff>
--- a/Mapa2.xlsx
+++ b/Mapa2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1Universidade\Computação Grafica\GAME3D2\Game3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB81C19-ABFE-4729-84DD-B2F954EFFABB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2055899-A52C-41BF-B2A1-A6A2E055A7B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{ADD39EA8-232B-4640-874C-2E799EA79373}"/>
   </bookViews>
@@ -49,7 +49,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,6 +74,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -87,12 +93,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,19 +416,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AF175D-EA1C-4544-ABA7-E5612A56070A}">
-  <dimension ref="A1:AX50"/>
+  <dimension ref="A1:AY51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="BC26" sqref="BC26"/>
+      <selection activeCell="BF24" sqref="BF24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="50" width="3" customWidth="1"/>
+    <col min="1" max="50" width="4.33203125" customWidth="1"/>
+    <col min="51" max="51" width="8.88671875" customWidth="1"/>
     <col min="53" max="53" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -570,8 +580,11 @@
       <c r="AX1" s="4">
         <v>0</v>
       </c>
+      <c r="AY1" s="5">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -722,8 +735,11 @@
       <c r="AX2" s="4">
         <v>0</v>
       </c>
+      <c r="AY2" s="5">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -874,8 +890,11 @@
       <c r="AX3" s="4">
         <v>0</v>
       </c>
+      <c r="AY3" s="5">
+        <v>48</v>
+      </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1026,8 +1045,11 @@
       <c r="AX4" s="4">
         <v>0</v>
       </c>
+      <c r="AY4" s="5">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -1178,8 +1200,11 @@
       <c r="AX5" s="4">
         <v>0</v>
       </c>
+      <c r="AY5" s="5">
+        <v>46</v>
+      </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -1330,8 +1355,11 @@
       <c r="AX6" s="4">
         <v>0</v>
       </c>
+      <c r="AY6" s="5">
+        <v>45</v>
+      </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -1482,8 +1510,11 @@
       <c r="AX7" s="4">
         <v>0</v>
       </c>
+      <c r="AY7" s="5">
+        <v>44</v>
+      </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -1634,8 +1665,11 @@
       <c r="AX8" s="4">
         <v>0</v>
       </c>
+      <c r="AY8" s="5">
+        <v>43</v>
+      </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -1786,8 +1820,11 @@
       <c r="AX9" s="4">
         <v>0</v>
       </c>
+      <c r="AY9" s="5">
+        <v>42</v>
+      </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -1938,8 +1975,11 @@
       <c r="AX10" s="4">
         <v>0</v>
       </c>
+      <c r="AY10" s="5">
+        <v>41</v>
+      </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -2090,8 +2130,11 @@
       <c r="AX11" s="4">
         <v>0</v>
       </c>
+      <c r="AY11" s="5">
+        <v>40</v>
+      </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -2242,8 +2285,11 @@
       <c r="AX12" s="4">
         <v>0</v>
       </c>
+      <c r="AY12" s="5">
+        <v>39</v>
+      </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -2394,8 +2440,11 @@
       <c r="AX13" s="4">
         <v>0</v>
       </c>
+      <c r="AY13" s="5">
+        <v>38</v>
+      </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>0</v>
       </c>
@@ -2546,8 +2595,11 @@
       <c r="AX14" s="4">
         <v>0</v>
       </c>
+      <c r="AY14" s="5">
+        <v>37</v>
+      </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>0</v>
       </c>
@@ -2698,8 +2750,11 @@
       <c r="AX15" s="4">
         <v>0</v>
       </c>
+      <c r="AY15" s="5">
+        <v>36</v>
+      </c>
     </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>0</v>
       </c>
@@ -2850,8 +2905,11 @@
       <c r="AX16" s="4">
         <v>0</v>
       </c>
+      <c r="AY16" s="5">
+        <v>35</v>
+      </c>
     </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -3002,8 +3060,11 @@
       <c r="AX17" s="4">
         <v>0</v>
       </c>
+      <c r="AY17" s="5">
+        <v>34</v>
+      </c>
     </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -3154,8 +3215,11 @@
       <c r="AX18" s="4">
         <v>0</v>
       </c>
+      <c r="AY18" s="5">
+        <v>33</v>
+      </c>
     </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -3306,8 +3370,11 @@
       <c r="AX19" s="4">
         <v>0</v>
       </c>
+      <c r="AY19" s="5">
+        <v>32</v>
+      </c>
     </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -3458,8 +3525,11 @@
       <c r="AX20" s="4">
         <v>0</v>
       </c>
+      <c r="AY20" s="5">
+        <v>31</v>
+      </c>
     </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>0</v>
       </c>
@@ -3610,8 +3680,11 @@
       <c r="AX21" s="4">
         <v>0</v>
       </c>
+      <c r="AY21" s="5">
+        <v>30</v>
+      </c>
     </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>0</v>
       </c>
@@ -3762,8 +3835,11 @@
       <c r="AX22" s="4">
         <v>0</v>
       </c>
+      <c r="AY22" s="5">
+        <v>29</v>
+      </c>
     </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>0</v>
       </c>
@@ -3914,8 +3990,11 @@
       <c r="AX23" s="4">
         <v>0</v>
       </c>
+      <c r="AY23" s="5">
+        <v>28</v>
+      </c>
     </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>0</v>
       </c>
@@ -4066,8 +4145,11 @@
       <c r="AX24" s="4">
         <v>0</v>
       </c>
+      <c r="AY24" s="5">
+        <v>27</v>
+      </c>
     </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>0</v>
       </c>
@@ -4218,8 +4300,11 @@
       <c r="AX25" s="4">
         <v>0</v>
       </c>
+      <c r="AY25" s="5">
+        <v>26</v>
+      </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>0</v>
       </c>
@@ -4370,8 +4455,11 @@
       <c r="AX26" s="4">
         <v>0</v>
       </c>
+      <c r="AY26" s="5">
+        <v>25</v>
+      </c>
     </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>0</v>
       </c>
@@ -4522,8 +4610,11 @@
       <c r="AX27" s="4">
         <v>0</v>
       </c>
+      <c r="AY27" s="5">
+        <v>24</v>
+      </c>
     </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -4674,8 +4765,11 @@
       <c r="AX28" s="4">
         <v>0</v>
       </c>
+      <c r="AY28" s="5">
+        <v>23</v>
+      </c>
     </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -4826,8 +4920,11 @@
       <c r="AX29" s="4">
         <v>0</v>
       </c>
+      <c r="AY29" s="5">
+        <v>22</v>
+      </c>
     </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -4978,8 +5075,11 @@
       <c r="AX30" s="4">
         <v>0</v>
       </c>
+      <c r="AY30" s="5">
+        <v>21</v>
+      </c>
     </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -5130,8 +5230,11 @@
       <c r="AX31" s="4">
         <v>0</v>
       </c>
+      <c r="AY31" s="5">
+        <v>20</v>
+      </c>
     </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>0</v>
       </c>
@@ -5282,8 +5385,11 @@
       <c r="AX32" s="4">
         <v>0</v>
       </c>
+      <c r="AY32" s="5">
+        <v>19</v>
+      </c>
     </row>
-    <row r="33" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>0</v>
       </c>
@@ -5434,8 +5540,11 @@
       <c r="AX33" s="4">
         <v>0</v>
       </c>
+      <c r="AY33" s="5">
+        <v>18</v>
+      </c>
     </row>
-    <row r="34" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>0</v>
       </c>
@@ -5586,8 +5695,11 @@
       <c r="AX34" s="4">
         <v>0</v>
       </c>
+      <c r="AY34" s="5">
+        <v>17</v>
+      </c>
     </row>
-    <row r="35" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>0</v>
       </c>
@@ -5738,8 +5850,11 @@
       <c r="AX35" s="4">
         <v>0</v>
       </c>
+      <c r="AY35" s="5">
+        <v>16</v>
+      </c>
     </row>
-    <row r="36" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>0</v>
       </c>
@@ -5890,8 +6005,11 @@
       <c r="AX36" s="4">
         <v>0</v>
       </c>
+      <c r="AY36" s="5">
+        <v>15</v>
+      </c>
     </row>
-    <row r="37" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>0</v>
       </c>
@@ -6042,8 +6160,11 @@
       <c r="AX37" s="4">
         <v>0</v>
       </c>
+      <c r="AY37" s="5">
+        <v>14</v>
+      </c>
     </row>
-    <row r="38" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>0</v>
       </c>
@@ -6194,8 +6315,11 @@
       <c r="AX38" s="4">
         <v>0</v>
       </c>
+      <c r="AY38" s="5">
+        <v>13</v>
+      </c>
     </row>
-    <row r="39" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>0</v>
       </c>
@@ -6346,8 +6470,11 @@
       <c r="AX39" s="4">
         <v>0</v>
       </c>
+      <c r="AY39" s="5">
+        <v>12</v>
+      </c>
     </row>
-    <row r="40" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -6498,8 +6625,11 @@
       <c r="AX40" s="4">
         <v>0</v>
       </c>
+      <c r="AY40" s="5">
+        <v>11</v>
+      </c>
     </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -6650,8 +6780,11 @@
       <c r="AX41" s="4">
         <v>0</v>
       </c>
+      <c r="AY41" s="5">
+        <v>10</v>
+      </c>
     </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -6802,8 +6935,11 @@
       <c r="AX42" s="4">
         <v>0</v>
       </c>
+      <c r="AY42" s="5">
+        <v>9</v>
+      </c>
     </row>
-    <row r="43" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -6954,8 +7090,11 @@
       <c r="AX43" s="4">
         <v>0</v>
       </c>
+      <c r="AY43" s="5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="44" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -7106,8 +7245,11 @@
       <c r="AX44" s="4">
         <v>0</v>
       </c>
+      <c r="AY44" s="5">
+        <v>7</v>
+      </c>
     </row>
-    <row r="45" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -7258,8 +7400,11 @@
       <c r="AX45" s="4">
         <v>0</v>
       </c>
+      <c r="AY45" s="5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="46" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -7410,8 +7555,11 @@
       <c r="AX46" s="4">
         <v>0</v>
       </c>
+      <c r="AY46" s="5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="47" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -7562,8 +7710,11 @@
       <c r="AX47" s="4">
         <v>0</v>
       </c>
+      <c r="AY47" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="48" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -7714,8 +7865,11 @@
       <c r="AX48" s="4">
         <v>0</v>
       </c>
+      <c r="AY48" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -7866,8 +8020,11 @@
       <c r="AX49" s="4">
         <v>0</v>
       </c>
+      <c r="AY49" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="50" spans="1:50" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -8017,6 +8174,161 @@
       </c>
       <c r="AX50" s="4">
         <v>0</v>
+      </c>
+      <c r="AY50" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:51" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6">
+        <v>1</v>
+      </c>
+      <c r="B51" s="5">
+        <v>2</v>
+      </c>
+      <c r="C51" s="5">
+        <v>3</v>
+      </c>
+      <c r="D51" s="5">
+        <v>4</v>
+      </c>
+      <c r="E51" s="7">
+        <v>5</v>
+      </c>
+      <c r="F51" s="7">
+        <v>6</v>
+      </c>
+      <c r="G51" s="7">
+        <v>7</v>
+      </c>
+      <c r="H51" s="7">
+        <v>8</v>
+      </c>
+      <c r="I51" s="7">
+        <v>9</v>
+      </c>
+      <c r="J51" s="7">
+        <v>10</v>
+      </c>
+      <c r="K51" s="7">
+        <v>11</v>
+      </c>
+      <c r="L51" s="7">
+        <v>12</v>
+      </c>
+      <c r="M51" s="7">
+        <v>13</v>
+      </c>
+      <c r="N51" s="7">
+        <v>14</v>
+      </c>
+      <c r="O51" s="7">
+        <v>15</v>
+      </c>
+      <c r="P51" s="7">
+        <v>16</v>
+      </c>
+      <c r="Q51" s="7">
+        <v>17</v>
+      </c>
+      <c r="R51" s="7">
+        <v>18</v>
+      </c>
+      <c r="S51" s="7">
+        <v>19</v>
+      </c>
+      <c r="T51" s="7">
+        <v>20</v>
+      </c>
+      <c r="U51" s="5">
+        <v>21</v>
+      </c>
+      <c r="V51" s="5">
+        <v>22</v>
+      </c>
+      <c r="W51" s="5">
+        <v>23</v>
+      </c>
+      <c r="X51" s="5">
+        <v>24</v>
+      </c>
+      <c r="Y51" s="5">
+        <v>25</v>
+      </c>
+      <c r="Z51" s="5">
+        <v>26</v>
+      </c>
+      <c r="AA51" s="5">
+        <v>27</v>
+      </c>
+      <c r="AB51" s="5">
+        <v>28</v>
+      </c>
+      <c r="AC51" s="5">
+        <v>29</v>
+      </c>
+      <c r="AD51" s="5">
+        <v>30</v>
+      </c>
+      <c r="AE51" s="5">
+        <v>31</v>
+      </c>
+      <c r="AF51" s="5">
+        <v>32</v>
+      </c>
+      <c r="AG51" s="5">
+        <v>33</v>
+      </c>
+      <c r="AH51" s="5">
+        <v>34</v>
+      </c>
+      <c r="AI51" s="5">
+        <v>35</v>
+      </c>
+      <c r="AJ51" s="5">
+        <v>36</v>
+      </c>
+      <c r="AK51" s="5">
+        <v>37</v>
+      </c>
+      <c r="AL51" s="5">
+        <v>38</v>
+      </c>
+      <c r="AM51" s="5">
+        <v>39</v>
+      </c>
+      <c r="AN51" s="5">
+        <v>40</v>
+      </c>
+      <c r="AO51" s="5">
+        <v>41</v>
+      </c>
+      <c r="AP51" s="5">
+        <v>42</v>
+      </c>
+      <c r="AQ51" s="5">
+        <v>43</v>
+      </c>
+      <c r="AR51" s="5">
+        <v>44</v>
+      </c>
+      <c r="AS51" s="5">
+        <v>45</v>
+      </c>
+      <c r="AT51" s="5">
+        <v>46</v>
+      </c>
+      <c r="AU51" s="5">
+        <v>47</v>
+      </c>
+      <c r="AV51" s="5">
+        <v>48</v>
+      </c>
+      <c r="AW51" s="5">
+        <v>49</v>
+      </c>
+      <c r="AX51" s="7">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Coelho pega as cenouras.
</commit_message>
<xml_diff>
--- a/Mapa2.xlsx
+++ b/Mapa2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1Universidade\Computação Grafica\GAME3D2\Game3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2055899-A52C-41BF-B2A1-A6A2E055A7B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EC82C0-FFB7-47D7-AF7C-5F9A9A0D9B1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{ADD39EA8-232B-4640-874C-2E799EA79373}"/>
+    <workbookView xWindow="11712" yWindow="552" windowWidth="10296" windowHeight="12336" xr2:uid="{ADD39EA8-232B-4640-874C-2E799EA79373}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,33 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Valores de X e Z devem ser contamos como -1 para adicionar ao jogo</t>
+  </si>
+  <si>
+    <t>Indica a posição da cenouras</t>
+  </si>
+  <si>
+    <t>Z        X</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -49,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,6 +101,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -93,15 +120,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AF175D-EA1C-4544-ABA7-E5612A56070A}">
-  <dimension ref="A1:AY51"/>
+  <dimension ref="A1:BF51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="BF24" sqref="BF24"/>
+    <sheetView tabSelected="1" topLeftCell="W4" zoomScale="58" workbookViewId="0">
+      <selection activeCell="AY51" sqref="AY51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,7 +461,7 @@
     <col min="53" max="53" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -584,7 +616,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -739,7 +771,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -749,7 +781,7 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="10">
         <v>1</v>
       </c>
       <c r="E3" s="1">
@@ -881,7 +913,7 @@
       <c r="AU3" s="1">
         <v>1</v>
       </c>
-      <c r="AV3" s="1">
+      <c r="AV3" s="10">
         <v>1</v>
       </c>
       <c r="AW3" s="1">
@@ -894,7 +926,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -1049,7 +1081,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -1204,7 +1236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -1358,8 +1390,11 @@
       <c r="AY6" s="5">
         <v>45</v>
       </c>
+      <c r="AZ6" s="8" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -1514,7 +1549,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -1669,7 +1704,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -1824,7 +1859,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -1979,7 +2014,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -2134,7 +2169,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -2288,8 +2323,12 @@
       <c r="AY12" s="5">
         <v>39</v>
       </c>
+      <c r="BA12" s="11"/>
+      <c r="BB12" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -2444,7 +2483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>0</v>
       </c>
@@ -2599,7 +2638,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>0</v>
       </c>
@@ -2754,7 +2793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>0</v>
       </c>
@@ -2909,7 +2948,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -3064,7 +3103,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -3219,7 +3258,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -3283,7 +3322,7 @@
       <c r="U19" s="1">
         <v>1</v>
       </c>
-      <c r="V19" s="1">
+      <c r="V19" s="9">
         <v>1</v>
       </c>
       <c r="W19" s="1">
@@ -3307,7 +3346,7 @@
       <c r="AC19" s="1">
         <v>1</v>
       </c>
-      <c r="AD19" s="1">
+      <c r="AD19" s="10">
         <v>1</v>
       </c>
       <c r="AE19" s="1">
@@ -3373,8 +3412,9 @@
       <c r="AY19" s="5">
         <v>32</v>
       </c>
+      <c r="BF19" s="12"/>
     </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -3529,7 +3569,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>0</v>
       </c>
@@ -3684,7 +3724,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>0</v>
       </c>
@@ -3839,7 +3879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>0</v>
       </c>
@@ -3994,7 +4034,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>0</v>
       </c>
@@ -4149,7 +4189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>0</v>
       </c>
@@ -4304,7 +4344,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>0</v>
       </c>
@@ -4459,7 +4499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>0</v>
       </c>
@@ -4614,7 +4654,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -4769,7 +4809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -4924,7 +4964,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -5079,7 +5119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -5234,7 +5274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>0</v>
       </c>
@@ -7101,7 +7141,7 @@
       <c r="B44" s="1">
         <v>1</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="10">
         <v>1</v>
       </c>
       <c r="D44" s="1">
@@ -8329,6 +8369,9 @@
       </c>
       <c r="AX51" s="7">
         <v>50</v>
+      </c>
+      <c r="AY51" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapa espelhado com os valores do lobo.andar
</commit_message>
<xml_diff>
--- a/Mapa2.xlsx
+++ b/Mapa2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1Universidade\Computação Grafica\GAME3D2\Game3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EC82C0-FFB7-47D7-AF7C-5F9A9A0D9B1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091CE5E1-B93F-4D38-AE2A-D3BACF8EECEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11712" yWindow="552" windowWidth="10296" windowHeight="12336" xr2:uid="{ADD39EA8-232B-4640-874C-2E799EA79373}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{ADD39EA8-232B-4640-874C-2E799EA79373}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Valores de X e Z devem ser contamos como -1 para adicionar ao jogo</t>
   </si>
@@ -40,6 +40,27 @@
   </si>
   <si>
     <t>Z        X</t>
+  </si>
+  <si>
+    <t>aumenta X</t>
+  </si>
+  <si>
+    <t>diminui X</t>
+  </si>
+  <si>
+    <t>diminui Z</t>
+  </si>
+  <si>
+    <t>aumenta Z</t>
+  </si>
+  <si>
+    <t>esquerda</t>
+  </si>
+  <si>
+    <t>direita</t>
+  </si>
+  <si>
+    <t>Andando valores:</t>
   </si>
 </sst>
 </file>
@@ -120,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -134,6 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,6 +171,1153 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>66260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>531839</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>137270</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F20E8FBC-B03E-4B58-AF1C-E83C3178F875}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="911087" y="12009782"/>
+          <a:ext cx="15142361" cy="12644010"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>307731</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>311638</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>13676</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector de Seta Reta 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08AE277C-F850-4C69-ABFF-390ECC5570D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16807962" y="14302154"/>
+          <a:ext cx="3907" cy="1830753"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>342901</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>123093</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector de Seta Reta 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{793B5176-42B6-41DD-A3C1-429BFD1A062C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16843132" y="16764000"/>
+          <a:ext cx="38099" cy="1588478"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA7C094-CE9F-47D4-9C4D-DE808B81288D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="19735800" y="18021300"/>
+          <a:ext cx="617220" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>84994</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector de Seta Reta 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5B90DFF-4903-449A-B95A-BDDF5DCC6B34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15764608" y="19017763"/>
+          <a:ext cx="1541584" cy="2929"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>542192</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>43962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>58615</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Conector de Seta Reta 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12745EA7-6154-4F7D-B7D7-897C9FD351F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="15811500" y="19855962"/>
+          <a:ext cx="1494692" cy="14653"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>463826</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>165653</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>480391</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>33131</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Conector de Seta Reta 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0294D8EF-6F43-466E-A818-48B7A00D6228}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="20888739" y="19397870"/>
+          <a:ext cx="16565" cy="1689652"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>480391</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>66260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>430695</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>99390</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Conector de Seta Reta 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AC23768-4658-4A32-9B61-C31C613DC955}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="19679478" y="20391782"/>
+          <a:ext cx="1789043" cy="33130"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>252939</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>58614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>231913</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>66260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Conector de Seta Reta 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E50E92E2-F5ED-4C5D-8CAF-9342FF300237}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20677852" y="20384136"/>
+          <a:ext cx="1204800" cy="7646"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>82826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>563217</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>115957</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector de Seta Reta 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24CB8676-50DE-415B-8D34-F2C05989FD37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="21650739" y="18403956"/>
+          <a:ext cx="1789043" cy="33131"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>198782</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>198782</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>33129</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Conector de Seta Reta 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB8BD92A-20E4-44F1-A879-9882D8E2D151}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="22462434" y="17376913"/>
+          <a:ext cx="0" cy="1159564"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>219808</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>91744</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>248478</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>66260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Conector de Seta Reta 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6E2E092-DDB8-4DC2-A98D-5CA1B3DAD3E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22483460" y="18230657"/>
+          <a:ext cx="28670" cy="1250038"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>202096</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>3315</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>516837</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>69573</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Conector de Seta Reta 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1576F4E-06DE-442A-BBAF-7628686DBA04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="19401183" y="17048924"/>
+          <a:ext cx="2153480" cy="66258"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>284922</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>53007</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>301487</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>135834</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Conector de Seta Reta 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8C5CC4A-88FF-4FB4-B617-08D45B76F3D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20709835" y="16916398"/>
+          <a:ext cx="16565" cy="1358349"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>268357</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>86139</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>289382</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>111622</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Conector de Seta Reta 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{488995EB-0E1A-455A-BC41-C97864FEA8AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="20693270" y="15856226"/>
+          <a:ext cx="21025" cy="1847657"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>500271</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>168966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>33130</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Conector de Seta Reta 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84C9147D-86C0-4C1C-B444-277C852E9169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19699358" y="21405575"/>
+          <a:ext cx="145772" cy="1835425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>57</xdr:col>
+      <xdr:colOff>36445</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>36443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>59</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Conector de Seta Reta 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E7895D9-E15F-414C-89DC-ED5384F2A184}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19235532" y="22184139"/>
+          <a:ext cx="1305338" cy="29818"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>347870</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>16564</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>256253</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>61927</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Conector de Seta Reta 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{067F4FDD-0DEC-4BBC-9602-EEB8C18B9209}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="18321131" y="22164260"/>
+          <a:ext cx="1747122" cy="45363"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>72887</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>155714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>139150</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>39755</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Conector de Seta Reta 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41EC125F-9C0D-4EFF-B03C-74F9C4D672FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7825409" y="19023497"/>
+          <a:ext cx="2153480" cy="66258"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>188844</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>23188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>205409</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>106016</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Conector de Seta Reta 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C5F7E55-FAE7-40A9-849D-7EC571AE79FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9134061" y="18890971"/>
+          <a:ext cx="16565" cy="1358349"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>172279</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>56321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>193304</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>81804</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="70" name="Conector de Seta Reta 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37719A72-C06A-457F-9B25-10FD04774645}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9117496" y="17830799"/>
+          <a:ext cx="21025" cy="1847657"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AF175D-EA1C-4544-ABA7-E5612A56070A}">
-  <dimension ref="A1:BF51"/>
+  <dimension ref="A1:BJ115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W4" zoomScale="58" workbookViewId="0">
-      <selection activeCell="AY51" sqref="AY51"/>
+    <sheetView tabSelected="1" zoomScale="34" workbookViewId="0">
+      <selection activeCell="BI129" sqref="BI129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8374,8 +9543,62 @@
         <v>2</v>
       </c>
     </row>
+    <row r="78" spans="53:53" x14ac:dyDescent="0.3">
+      <c r="BA78" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="55:62" x14ac:dyDescent="0.3">
+      <c r="BI84" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="BJ84" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="55:62" x14ac:dyDescent="0.3">
+      <c r="BC85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="55:62" x14ac:dyDescent="0.3">
+      <c r="BC87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="55:56" x14ac:dyDescent="0.3">
+      <c r="BC99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="55:56" x14ac:dyDescent="0.3">
+      <c r="BC102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="55:56" x14ac:dyDescent="0.3">
+      <c r="BD107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="55:56" x14ac:dyDescent="0.3">
+      <c r="BD109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="55:56" x14ac:dyDescent="0.3">
+      <c r="BD112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="56:56" x14ac:dyDescent="0.3">
+      <c r="BD115">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mapa sem pontas. Cenouras reposicionadas.
</commit_message>
<xml_diff>
--- a/Mapa2.xlsx
+++ b/Mapa2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1Universidade\Computação Grafica\GAME3D2\Game3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091CE5E1-B93F-4D38-AE2A-D3BACF8EECEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCCE1C4-D6A6-41F9-92FE-BEF9436031D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{ADD39EA8-232B-4640-874C-2E799EA79373}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Valores de X e Z devem ser contamos como -1 para adicionar ao jogo</t>
   </si>
@@ -62,6 +62,51 @@
   <si>
     <t>Andando valores:</t>
   </si>
+  <si>
+    <t>0 0</t>
+  </si>
+  <si>
+    <t>1 0</t>
+  </si>
+  <si>
+    <t>2 0</t>
+  </si>
+  <si>
+    <t>0 1</t>
+  </si>
+  <si>
+    <t>1 1</t>
+  </si>
+  <si>
+    <t>2 1</t>
+  </si>
+  <si>
+    <t>2 2</t>
+  </si>
+  <si>
+    <t>1 2</t>
+  </si>
+  <si>
+    <t>0 2</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>5 22</t>
+  </si>
+  <si>
+    <t>4 21</t>
+  </si>
+  <si>
+    <t>6 22</t>
+  </si>
+  <si>
+    <t>4 22</t>
+  </si>
 </sst>
 </file>
 
@@ -91,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,8 +173,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -137,11 +188,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -151,11 +217,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -175,50 +243,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>16565</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>66260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>531839</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>137270</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F20E8FBC-B03E-4B58-AF1C-E83C3178F875}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="911087" y="12009782"/>
-          <a:ext cx="15142361" cy="12644010"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>53</xdr:col>
@@ -352,7 +376,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1155,15 +1179,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>72887</xdr:colOff>
+      <xdr:colOff>36285</xdr:colOff>
       <xdr:row>102</xdr:row>
       <xdr:rowOff>155714</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>139150</xdr:colOff>
+      <xdr:colOff>139151</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>39755</xdr:rowOff>
+      <xdr:rowOff>12096</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1178,8 +1202,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7825409" y="19023497"/>
-          <a:ext cx="2153480" cy="66258"/>
+          <a:off x="7898190" y="18939619"/>
+          <a:ext cx="2219532" cy="37810"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1315,6 +1339,174 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="Text Box 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{417736CE-D19B-4E65-AD00-21F4DB489A9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="381000" cy="251460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+              <a:cs typeface="Calibri"/>
+            </a:rPr>
+            <a:t>printf("LOBO ANDANDO X BAIXO");</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>242999</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>149980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>286069</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>152909</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Conector de Seta Reta 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5D44397-3C1A-447B-B250-D3D2ADDEBB80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8591869" y="19017763"/>
+          <a:ext cx="1533939" cy="2929"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="76200">
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>20461</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>145472</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>206554</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57B783AE-CE04-4647-9FBE-9DEBE3E5284D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="20461" y="12918497"/>
+          <a:ext cx="10225443" cy="6655377"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1619,8 +1811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AF175D-EA1C-4544-ABA7-E5612A56070A}">
   <dimension ref="A1:BJ115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="34" workbookViewId="0">
-      <selection activeCell="BI129" sqref="BI129"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" workbookViewId="0">
+      <selection activeCell="AQ64" sqref="AQ64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1637,17 +1829,17 @@
       <c r="B1" s="3">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1</v>
+      <c r="C1" s="3">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3">
+        <v>0</v>
       </c>
       <c r="G1" s="3">
         <v>0</v>
@@ -1792,17 +1984,17 @@
       <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
@@ -1947,17 +2139,17 @@
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -2082,7 +2274,7 @@
       <c r="AU3" s="1">
         <v>1</v>
       </c>
-      <c r="AV3" s="10">
+      <c r="AV3" s="9">
         <v>1</v>
       </c>
       <c r="AW3" s="1">
@@ -2102,17 +2294,17 @@
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -2257,17 +2449,17 @@
       <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -3492,7 +3684,7 @@
       <c r="AY12" s="5">
         <v>39</v>
       </c>
-      <c r="BA12" s="11"/>
+      <c r="BA12" s="10"/>
       <c r="BB12" t="s">
         <v>1</v>
       </c>
@@ -4491,7 +4683,7 @@
       <c r="U19" s="1">
         <v>1</v>
       </c>
-      <c r="V19" s="9">
+      <c r="V19" s="1">
         <v>1</v>
       </c>
       <c r="W19" s="1">
@@ -4515,7 +4707,7 @@
       <c r="AC19" s="1">
         <v>1</v>
       </c>
-      <c r="AD19" s="10">
+      <c r="AD19" s="9">
         <v>1</v>
       </c>
       <c r="AE19" s="1">
@@ -4581,7 +4773,7 @@
       <c r="AY19" s="5">
         <v>32</v>
       </c>
-      <c r="BF19" s="12"/>
+      <c r="BF19" s="11"/>
     </row>
     <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
@@ -4590,17 +4782,17 @@
       <c r="B20" s="3">
         <v>0</v>
       </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
@@ -4745,17 +4937,17 @@
       <c r="B21" s="3">
         <v>0</v>
       </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0</v>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
@@ -4900,17 +5092,17 @@
       <c r="B22" s="3">
         <v>0</v>
       </c>
-      <c r="C22" s="3">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>2</v>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
       </c>
       <c r="G22" s="2">
         <v>2</v>
@@ -5055,17 +5247,17 @@
       <c r="B23" s="3">
         <v>0</v>
       </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>2</v>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
       </c>
       <c r="G23" s="2">
         <v>2</v>
@@ -5210,17 +5402,17 @@
       <c r="B24" s="3">
         <v>0</v>
       </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2</v>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
       </c>
       <c r="G24" s="2">
         <v>2</v>
@@ -5365,17 +5557,17 @@
       <c r="B25" s="3">
         <v>0</v>
       </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>0</v>
-      </c>
-      <c r="F25" s="2">
-        <v>2</v>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
       </c>
       <c r="G25" s="2">
         <v>2</v>
@@ -5520,17 +5712,17 @@
       <c r="B26" s="3">
         <v>0</v>
       </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0</v>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
       </c>
       <c r="G26" s="3">
         <v>0</v>
@@ -5675,17 +5867,17 @@
       <c r="B27" s="3">
         <v>0</v>
       </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <v>0</v>
-      </c>
-      <c r="E27" s="3">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0</v>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
       </c>
       <c r="G27" s="3">
         <v>0</v>
@@ -5824,11 +6016,11 @@
       </c>
     </row>
     <row r="28" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
+      <c r="A28" s="3">
+        <v>0</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -5979,11 +6171,11 @@
       </c>
     </row>
     <row r="29" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>1</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
+      <c r="A29" s="3">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -6134,11 +6326,11 @@
       </c>
     </row>
     <row r="30" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>1</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1</v>
+      <c r="A30" s="3">
+        <v>0</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -6289,11 +6481,11 @@
       </c>
     </row>
     <row r="31" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>1</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1</v>
+      <c r="A31" s="3">
+        <v>0</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
@@ -6450,17 +6642,17 @@
       <c r="B32" s="4">
         <v>0</v>
       </c>
-      <c r="C32" s="4">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0</v>
-      </c>
-      <c r="E32" s="4">
-        <v>0</v>
-      </c>
-      <c r="F32" s="4">
-        <v>0</v>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
       </c>
       <c r="G32" s="4">
         <v>0</v>
@@ -6605,17 +6797,17 @@
       <c r="B33" s="4">
         <v>0</v>
       </c>
-      <c r="C33" s="4">
-        <v>0</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0</v>
-      </c>
-      <c r="E33" s="4">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4">
-        <v>0</v>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
       </c>
       <c r="G33" s="4">
         <v>0</v>
@@ -6760,17 +6952,17 @@
       <c r="B34" s="4">
         <v>0</v>
       </c>
-      <c r="C34" s="4">
-        <v>0</v>
-      </c>
-      <c r="D34" s="4">
-        <v>0</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0</v>
-      </c>
-      <c r="F34" s="4">
-        <v>0</v>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
       </c>
       <c r="G34" s="4">
         <v>0</v>
@@ -6915,17 +7107,17 @@
       <c r="B35" s="4">
         <v>0</v>
       </c>
-      <c r="C35" s="4">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4">
-        <v>0</v>
-      </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="F35" s="4">
-        <v>0</v>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
       </c>
       <c r="G35" s="4">
         <v>0</v>
@@ -7070,17 +7262,17 @@
       <c r="B36" s="4">
         <v>0</v>
       </c>
-      <c r="C36" s="4">
-        <v>0</v>
-      </c>
-      <c r="D36" s="4">
-        <v>0</v>
-      </c>
-      <c r="E36" s="4">
-        <v>0</v>
-      </c>
-      <c r="F36" s="4">
-        <v>0</v>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
       </c>
       <c r="G36" s="4">
         <v>0</v>
@@ -7225,17 +7417,17 @@
       <c r="B37" s="4">
         <v>0</v>
       </c>
-      <c r="C37" s="4">
-        <v>0</v>
-      </c>
-      <c r="D37" s="4">
-        <v>0</v>
-      </c>
-      <c r="E37" s="4">
-        <v>0</v>
-      </c>
-      <c r="F37" s="4">
-        <v>0</v>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
       </c>
       <c r="G37" s="4">
         <v>0</v>
@@ -7380,17 +7572,17 @@
       <c r="B38" s="4">
         <v>0</v>
       </c>
-      <c r="C38" s="4">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0</v>
-      </c>
-      <c r="E38" s="4">
-        <v>0</v>
-      </c>
-      <c r="F38" s="4">
-        <v>0</v>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
       </c>
       <c r="G38" s="4">
         <v>0</v>
@@ -7535,17 +7727,17 @@
       <c r="B39" s="4">
         <v>0</v>
       </c>
-      <c r="C39" s="4">
-        <v>0</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0</v>
-      </c>
-      <c r="E39" s="4">
-        <v>0</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0</v>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
       </c>
       <c r="G39" s="4">
         <v>0</v>
@@ -7684,11 +7876,11 @@
       </c>
     </row>
     <row r="40" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>1</v>
-      </c>
-      <c r="B40" s="1">
-        <v>1</v>
+      <c r="A40" s="4">
+        <v>0</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
@@ -7839,11 +8031,11 @@
       </c>
     </row>
     <row r="41" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>1</v>
-      </c>
-      <c r="B41" s="1">
-        <v>1</v>
+      <c r="A41" s="4">
+        <v>0</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
@@ -7994,11 +8186,11 @@
       </c>
     </row>
     <row r="42" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>1</v>
-      </c>
-      <c r="B42" s="1">
-        <v>1</v>
+      <c r="A42" s="4">
+        <v>0</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
@@ -8149,11 +8341,11 @@
       </c>
     </row>
     <row r="43" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>1</v>
-      </c>
-      <c r="B43" s="1">
-        <v>1</v>
+      <c r="A43" s="4">
+        <v>0</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
@@ -8304,17 +8496,17 @@
       </c>
     </row>
     <row r="44" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>1</v>
-      </c>
-      <c r="B44" s="1">
-        <v>1</v>
-      </c>
-      <c r="C44" s="10">
-        <v>1</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1</v>
+      <c r="A44" s="4">
+        <v>0</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
       </c>
       <c r="E44" s="4">
         <v>0</v>
@@ -8459,17 +8651,17 @@
       </c>
     </row>
     <row r="45" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>1</v>
-      </c>
-      <c r="B45" s="1">
-        <v>1</v>
-      </c>
-      <c r="C45" s="1">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
+      <c r="A45" s="4">
+        <v>0</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
       </c>
       <c r="E45" s="4">
         <v>0</v>
@@ -8614,17 +8806,17 @@
       </c>
     </row>
     <row r="46" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>1</v>
-      </c>
-      <c r="B46" s="1">
-        <v>1</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1</v>
-      </c>
-      <c r="D46" s="1">
-        <v>1</v>
+      <c r="A46" s="4">
+        <v>0</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
       </c>
       <c r="E46" s="4">
         <v>0</v>
@@ -8769,17 +8961,17 @@
       </c>
     </row>
     <row r="47" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>1</v>
-      </c>
-      <c r="B47" s="1">
-        <v>1</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
+      <c r="A47" s="4">
+        <v>0</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
       </c>
       <c r="E47" s="4">
         <v>0</v>
@@ -8924,17 +9116,17 @@
       </c>
     </row>
     <row r="48" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>1</v>
-      </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
+      <c r="A48" s="4">
+        <v>0</v>
+      </c>
+      <c r="B48" s="4">
+        <v>0</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
       </c>
       <c r="E48" s="4">
         <v>0</v>
@@ -9079,17 +9271,17 @@
       </c>
     </row>
     <row r="49" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>1</v>
-      </c>
-      <c r="B49" s="1">
-        <v>1</v>
-      </c>
-      <c r="C49" s="1">
-        <v>1</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
+      <c r="A49" s="4">
+        <v>0</v>
+      </c>
+      <c r="B49" s="4">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4">
+        <v>0</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
       </c>
       <c r="E49" s="4">
         <v>0</v>
@@ -9139,17 +9331,17 @@
       <c r="T49" s="4">
         <v>0</v>
       </c>
-      <c r="U49" s="1">
-        <v>1</v>
-      </c>
-      <c r="V49" s="1">
-        <v>1</v>
-      </c>
-      <c r="W49" s="1">
-        <v>1</v>
-      </c>
-      <c r="X49" s="1">
-        <v>1</v>
+      <c r="U49" s="4">
+        <v>0</v>
+      </c>
+      <c r="V49" s="4">
+        <v>0</v>
+      </c>
+      <c r="W49" s="4">
+        <v>0</v>
+      </c>
+      <c r="X49" s="4">
+        <v>0</v>
       </c>
       <c r="Y49" s="4">
         <v>0</v>
@@ -9234,17 +9426,17 @@
       </c>
     </row>
     <row r="50" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>1</v>
-      </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1">
-        <v>1</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
+      <c r="A50" s="4">
+        <v>0</v>
+      </c>
+      <c r="B50" s="4">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
       </c>
       <c r="E50" s="4">
         <v>0</v>
@@ -9294,17 +9486,17 @@
       <c r="T50" s="4">
         <v>0</v>
       </c>
-      <c r="U50" s="1">
-        <v>1</v>
-      </c>
-      <c r="V50" s="1">
-        <v>1</v>
-      </c>
-      <c r="W50" s="1">
-        <v>1</v>
-      </c>
-      <c r="X50" s="1">
-        <v>1</v>
+      <c r="U50" s="4">
+        <v>0</v>
+      </c>
+      <c r="V50" s="4">
+        <v>0</v>
+      </c>
+      <c r="W50" s="4">
+        <v>0</v>
+      </c>
+      <c r="X50" s="4">
+        <v>0</v>
       </c>
       <c r="Y50" s="4">
         <v>0</v>
@@ -9543,16 +9735,170 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="53:53" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="X58" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="X59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="U60" t="s">
+        <v>19</v>
+      </c>
+      <c r="V60" t="s">
+        <v>20</v>
+      </c>
+      <c r="X60">
+        <v>-1</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="U61">
+        <v>1</v>
+      </c>
+      <c r="V61">
+        <v>-1</v>
+      </c>
+      <c r="X61">
+        <v>0</v>
+      </c>
+      <c r="Z61">
+        <v>-1</v>
+      </c>
+      <c r="AA61">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="W62" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="X62" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y62" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="U63">
+        <v>1</v>
+      </c>
+      <c r="V63">
+        <v>0</v>
+      </c>
+      <c r="W63" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="X63" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y63" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z63">
+        <v>-1</v>
+      </c>
+      <c r="AA63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="W64" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="X64" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y64" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="21:53" x14ac:dyDescent="0.3">
+      <c r="U65">
+        <v>1</v>
+      </c>
+      <c r="V65">
+        <v>1</v>
+      </c>
+      <c r="X65">
+        <v>0</v>
+      </c>
+      <c r="Z65">
+        <v>-1</v>
+      </c>
+      <c r="AA65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="21:53" x14ac:dyDescent="0.3">
+      <c r="X66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="21:53" x14ac:dyDescent="0.3">
+      <c r="X67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="21:53" x14ac:dyDescent="0.3">
+      <c r="X68" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="21:53" x14ac:dyDescent="0.3">
+      <c r="W72" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="X72" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y72" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="21:53" x14ac:dyDescent="0.3">
+      <c r="W73" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="X73" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y73" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="21:53" x14ac:dyDescent="0.3">
+      <c r="W74" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="X74" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y74" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="21:53" x14ac:dyDescent="0.3">
       <c r="BA78" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="84" spans="55:62" x14ac:dyDescent="0.3">
-      <c r="BI84" s="13" t="s">
+      <c r="BI84" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BJ84" s="11" t="s">
+      <c r="BJ84" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -9566,27 +9912,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="55:56" x14ac:dyDescent="0.3">
+    <row r="99" spans="38:56" x14ac:dyDescent="0.3">
       <c r="BC99" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="55:56" x14ac:dyDescent="0.3">
+    <row r="102" spans="38:56" x14ac:dyDescent="0.3">
       <c r="BC102">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="55:56" x14ac:dyDescent="0.3">
+    <row r="107" spans="38:56" x14ac:dyDescent="0.3">
       <c r="BD107" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="55:56" x14ac:dyDescent="0.3">
+    <row r="109" spans="38:56" x14ac:dyDescent="0.3">
+      <c r="AL109" s="12"/>
+      <c r="AM109">
+        <v>0</v>
+      </c>
       <c r="BD109">
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="55:56" x14ac:dyDescent="0.3">
+    <row r="110" spans="38:56" x14ac:dyDescent="0.3">
+      <c r="AL110" s="14"/>
+      <c r="AM110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="38:56" x14ac:dyDescent="0.3">
+      <c r="AL111" s="10"/>
+      <c r="AM111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="38:56" x14ac:dyDescent="0.3">
+      <c r="AL112" s="15"/>
+      <c r="AM112">
+        <v>3</v>
+      </c>
       <c r="BD112" t="s">
         <v>6</v>
       </c>

</xml_diff>